<commit_message>
fixed file input styling and indexing bugs.
</commit_message>
<xml_diff>
--- a/test-1.xlsx
+++ b/test-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aadig\repos\AIFracing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF66763E-433E-4A1D-8F13-BFEEDA7D4F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF551CB-DFD1-4F51-86E2-32722F2CB017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11835" xr2:uid="{BB6F3B86-ECC9-4F38-9376-CB7374BDE834}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BB6F3B86-ECC9-4F38-9376-CB7374BDE834}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -143,17 +143,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -161,8 +161,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -506,290 +518,344 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01068E15-9364-4A9F-B466-2D832AB5180B}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6">
+        <v>12000</v>
+      </c>
+      <c r="F2" s="6">
+        <v>50</v>
+      </c>
+      <c r="G2" s="6">
+        <v>90</v>
+      </c>
+      <c r="H2" s="6">
+        <v>240</v>
+      </c>
+      <c r="I2" s="7">
+        <v>1800</v>
+      </c>
+      <c r="J2" s="6">
+        <v>36</v>
+      </c>
+      <c r="K2" s="7">
+        <v>8640</v>
+      </c>
+      <c r="L2" s="7">
+        <v>432000</v>
+      </c>
+      <c r="M2" s="6">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6">
+        <v>12400</v>
+      </c>
+      <c r="F3" s="6">
+        <v>62</v>
+      </c>
+      <c r="G3" s="6">
+        <v>90</v>
+      </c>
+      <c r="H3" s="6">
+        <v>200</v>
+      </c>
+      <c r="I3" s="7">
+        <v>2000</v>
+      </c>
+      <c r="J3" s="6">
+        <v>40</v>
+      </c>
+      <c r="K3" s="7">
+        <v>8000</v>
+      </c>
+      <c r="L3" s="7">
+        <v>400000</v>
+      </c>
+      <c r="M3" s="6">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="6">
+        <v>12400</v>
+      </c>
+      <c r="F4" s="6">
+        <v>62</v>
+      </c>
+      <c r="G4" s="6">
+        <v>90</v>
+      </c>
+      <c r="H4" s="6">
+        <v>200</v>
+      </c>
+      <c r="I4" s="7">
+        <v>2400</v>
+      </c>
+      <c r="J4" s="6">
+        <v>45</v>
+      </c>
+      <c r="K4" s="7">
+        <v>9000</v>
+      </c>
+      <c r="L4" s="7">
+        <v>480000</v>
+      </c>
+      <c r="M4" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6">
+        <v>15000</v>
+      </c>
+      <c r="F5" s="6">
+        <v>75</v>
+      </c>
+      <c r="G5" s="6">
+        <v>90</v>
+      </c>
+      <c r="H5" s="6">
+        <v>200</v>
+      </c>
+      <c r="I5" s="7">
+        <v>2400</v>
+      </c>
+      <c r="J5" s="6">
+        <v>45</v>
+      </c>
+      <c r="K5" s="7">
+        <v>9000</v>
+      </c>
+      <c r="L5" s="7">
+        <v>480000</v>
+      </c>
+      <c r="M5" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="6">
+        <v>18000</v>
+      </c>
+      <c r="F6" s="6">
+        <v>90</v>
+      </c>
+      <c r="G6" s="6">
+        <v>90</v>
+      </c>
+      <c r="H6" s="6">
+        <v>200</v>
+      </c>
+      <c r="I6" s="7">
+        <v>2500</v>
+      </c>
+      <c r="J6" s="6">
+        <v>50</v>
+      </c>
+      <c r="K6" s="7">
+        <v>10000</v>
+      </c>
+      <c r="L6" s="7">
+        <v>500000</v>
+      </c>
+      <c r="M6" s="6">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="E7" s="6">
+        <v>18000</v>
+      </c>
+      <c r="F7" s="6">
+        <v>90</v>
+      </c>
+      <c r="G7" s="6">
+        <v>90</v>
+      </c>
+      <c r="H7" s="6">
+        <v>200</v>
+      </c>
+      <c r="I7" s="7">
+        <v>3000</v>
+      </c>
+      <c r="J7" s="6">
+        <v>60</v>
+      </c>
+      <c r="K7" s="7">
         <v>12000</v>
       </c>
-      <c r="C5" s="2">
-        <v>12400</v>
-      </c>
-      <c r="D5" s="2">
-        <v>12400</v>
-      </c>
-      <c r="E5" s="2">
-        <v>15000</v>
-      </c>
-      <c r="F5" s="2">
-        <v>18000</v>
-      </c>
-      <c r="G5" s="2">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2">
-        <v>50</v>
-      </c>
-      <c r="C6" s="2">
-        <v>62</v>
-      </c>
-      <c r="D6" s="2">
-        <v>62</v>
-      </c>
-      <c r="E6" s="2">
-        <v>75</v>
-      </c>
-      <c r="F6" s="2">
-        <v>90</v>
-      </c>
-      <c r="G6" s="2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2">
-        <v>90</v>
-      </c>
-      <c r="C7" s="2">
-        <v>90</v>
-      </c>
-      <c r="D7" s="2">
-        <v>90</v>
-      </c>
-      <c r="E7" s="2">
-        <v>90</v>
-      </c>
-      <c r="F7" s="2">
-        <v>90</v>
-      </c>
-      <c r="G7" s="2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="2">
-        <v>240</v>
-      </c>
-      <c r="C8" s="2">
-        <v>200</v>
-      </c>
-      <c r="D8" s="2">
-        <v>200</v>
-      </c>
-      <c r="E8" s="2">
-        <v>200</v>
-      </c>
-      <c r="F8" s="2">
-        <v>200</v>
-      </c>
-      <c r="G8" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1800</v>
-      </c>
-      <c r="C9" s="3">
-        <v>2000</v>
-      </c>
-      <c r="D9" s="3">
-        <v>2400</v>
-      </c>
-      <c r="E9" s="3">
-        <v>2400</v>
-      </c>
-      <c r="F9" s="3">
-        <v>2500</v>
-      </c>
-      <c r="G9" s="3">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2">
-        <v>36</v>
-      </c>
-      <c r="C10" s="2">
-        <v>40</v>
-      </c>
-      <c r="D10" s="2">
-        <v>45</v>
-      </c>
-      <c r="E10" s="2">
-        <v>45</v>
-      </c>
-      <c r="F10" s="2">
-        <v>50</v>
-      </c>
-      <c r="G10" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="3">
-        <v>8640</v>
-      </c>
-      <c r="C11" s="3">
-        <v>8000</v>
-      </c>
-      <c r="D11" s="3">
-        <v>9000</v>
-      </c>
-      <c r="E11" s="3">
-        <v>9000</v>
-      </c>
-      <c r="F11" s="3">
-        <v>10000</v>
-      </c>
-      <c r="G11" s="3">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="3">
-        <v>432000</v>
-      </c>
-      <c r="C12" s="3">
-        <v>400000</v>
-      </c>
-      <c r="D12" s="3">
-        <v>480000</v>
-      </c>
-      <c r="E12" s="3">
-        <v>480000</v>
-      </c>
-      <c r="F12" s="3">
-        <v>500000</v>
-      </c>
-      <c r="G12" s="3">
+      <c r="L7" s="7">
         <v>600000</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="2">
-        <v>96</v>
-      </c>
-      <c r="C13" s="2">
-        <v>89</v>
-      </c>
-      <c r="D13" s="2">
-        <v>100</v>
-      </c>
-      <c r="E13" s="2">
-        <v>100</v>
-      </c>
-      <c r="F13" s="2">
-        <v>111</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="M7" s="6">
         <v>133</v>
       </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>